<commit_message>
learning to read data
</commit_message>
<xml_diff>
--- a/xauusd_4_hourly.xlsx
+++ b/xauusd_4_hourly.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="208" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1808,7 +1808,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1987,8 +1986,8 @@
   </sheetPr>
   <dimension ref="A1:S452"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="S5" activeCellId="0" pane="topLeft" sqref="S5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2299,6 +2298,7 @@
         <v>0.5</v>
       </c>
       <c r="N6" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M6)</f>
         <v>448</v>
       </c>
       <c r="O6" s="0" t="n">
@@ -2359,6 +2359,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M7)</f>
         <v>440</v>
       </c>
       <c r="O7" s="0" t="n">
@@ -2421,6 +2422,7 @@
         <v>1.5</v>
       </c>
       <c r="N8" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M8)</f>
         <v>408</v>
       </c>
       <c r="O8" s="0" t="n">
@@ -2489,6 +2491,7 @@
         <v>2</v>
       </c>
       <c r="N9" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M9)</f>
         <v>368</v>
       </c>
       <c r="O9" s="0" t="n">
@@ -2557,6 +2560,7 @@
         <v>2.5</v>
       </c>
       <c r="N10" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M10)</f>
         <v>326</v>
       </c>
       <c r="O10" s="0" t="n">
@@ -2625,6 +2629,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M11)</f>
         <v>271</v>
       </c>
       <c r="O11" s="0" t="n">
@@ -2693,6 +2698,7 @@
         <v>3.5</v>
       </c>
       <c r="N12" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M12)</f>
         <v>239</v>
       </c>
       <c r="O12" s="0" t="n">
@@ -2761,6 +2767,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M13)</f>
         <v>201</v>
       </c>
       <c r="O13" s="0" t="n">
@@ -2829,6 +2836,7 @@
         <v>4.5</v>
       </c>
       <c r="N14" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M14)</f>
         <v>172</v>
       </c>
       <c r="O14" s="0" t="n">
@@ -2897,6 +2905,7 @@
         <v>5</v>
       </c>
       <c r="N15" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M15)</f>
         <v>153</v>
       </c>
       <c r="O15" s="0" t="n">
@@ -2965,6 +2974,7 @@
         <v>5.5</v>
       </c>
       <c r="N16" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M16)</f>
         <v>128</v>
       </c>
       <c r="P16" s="4" t="n">
@@ -3024,6 +3034,7 @@
         <v>6</v>
       </c>
       <c r="N17" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M17)</f>
         <v>109</v>
       </c>
       <c r="P17" s="4" t="n">
@@ -3083,6 +3094,7 @@
         <v>6.5</v>
       </c>
       <c r="N18" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M18)</f>
         <v>97</v>
       </c>
       <c r="P18" s="4" t="n">
@@ -3142,6 +3154,7 @@
         <v>7</v>
       </c>
       <c r="N19" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M19)</f>
         <v>81</v>
       </c>
       <c r="P19" s="4" t="n">
@@ -3197,6 +3210,21 @@
         <f aca="false">IF(H20&lt;I20,H20, I20)</f>
         <v>1.06000000000017</v>
       </c>
+      <c r="M20" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M20)</f>
+        <v>67</v>
+      </c>
+      <c r="P20" s="4" t="n">
+        <f aca="false">N20 / $O$3</f>
+        <v>0.148558758314856</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <f aca="false">N20 / N17</f>
+        <v>0.614678899082569</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="3" t="s">
@@ -3240,6 +3268,21 @@
         <f aca="false">IF(H21&lt;I21,H21, I21)</f>
         <v>0.759999999999991</v>
       </c>
+      <c r="M21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M21)</f>
+        <v>56</v>
+      </c>
+      <c r="P21" s="4" t="n">
+        <f aca="false">N21 / $O$3</f>
+        <v>0.124168514412417</v>
+      </c>
+      <c r="R21" s="4" t="n">
+        <f aca="false">N21 / N18</f>
+        <v>0.577319587628866</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="3" t="s">
@@ -3283,6 +3326,21 @@
         <f aca="false">IF(H22&lt;I22,H22, I22)</f>
         <v>1.56999999999994</v>
       </c>
+      <c r="M22" s="0" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M22)</f>
+        <v>49</v>
+      </c>
+      <c r="P22" s="4" t="n">
+        <f aca="false">N22 / $O$3</f>
+        <v>0.108647450110865</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <f aca="false">N22 / N19</f>
+        <v>0.604938271604938</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="3" t="s">
@@ -3326,6 +3384,21 @@
         <f aca="false">IF(H23&lt;I23,H23, I23)</f>
         <v>0</v>
       </c>
+      <c r="M23" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M23)</f>
+        <v>40</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <f aca="false">N23 / $O$3</f>
+        <v>0.0886917960088692</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <f aca="false">N23 / N20</f>
+        <v>0.597014925373134</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="3" t="s">
@@ -3369,6 +3442,21 @@
         <f aca="false">IF(H24&lt;I24,H24, I24)</f>
         <v>1.32999999999993</v>
       </c>
+      <c r="M24" s="0" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M24)</f>
+        <v>32</v>
+      </c>
+      <c r="P24" s="4" t="n">
+        <f aca="false">N24 / $O$3</f>
+        <v>0.0709534368070953</v>
+      </c>
+      <c r="R24" s="4" t="n">
+        <f aca="false">N24 / N21</f>
+        <v>0.571428571428571</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="3" t="s">
@@ -3412,6 +3500,21 @@
         <f aca="false">IF(H25&lt;I25,H25, I25)</f>
         <v>1.42000000000007</v>
       </c>
+      <c r="M25" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M25)</f>
+        <v>27</v>
+      </c>
+      <c r="P25" s="4" t="n">
+        <f aca="false">N25 / $O$3</f>
+        <v>0.0598669623059867</v>
+      </c>
+      <c r="R25" s="4" t="n">
+        <f aca="false">N25 / N22</f>
+        <v>0.551020408163265</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="3" t="s">
@@ -3455,6 +3558,21 @@
         <f aca="false">IF(H26&lt;I26,H26, I26)</f>
         <v>0.0399999999999636</v>
       </c>
+      <c r="M26" s="0" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M26)</f>
+        <v>26</v>
+      </c>
+      <c r="P26" s="4" t="n">
+        <f aca="false">N26 / $O$3</f>
+        <v>0.057649667405765</v>
+      </c>
+      <c r="R26" s="4" t="n">
+        <f aca="false">N26 / N23</f>
+        <v>0.65</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="3" t="s">
@@ -3498,6 +3616,21 @@
         <f aca="false">IF(H27&lt;I27,H27, I27)</f>
         <v>1.37999999999988</v>
       </c>
+      <c r="M27" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M27)</f>
+        <v>26</v>
+      </c>
+      <c r="P27" s="4" t="n">
+        <f aca="false">N27 / $O$3</f>
+        <v>0.057649667405765</v>
+      </c>
+      <c r="R27" s="4" t="n">
+        <f aca="false">N27 / N24</f>
+        <v>0.8125</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="3" t="s">
@@ -3541,6 +3674,21 @@
         <f aca="false">IF(H28&lt;I28,H28, I28)</f>
         <v>0</v>
       </c>
+      <c r="M28" s="0" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M28)</f>
+        <v>22</v>
+      </c>
+      <c r="P28" s="4" t="n">
+        <f aca="false">N28 / $O$3</f>
+        <v>0.0487804878048781</v>
+      </c>
+      <c r="R28" s="4" t="n">
+        <f aca="false">N28 / N25</f>
+        <v>0.814814814814815</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="3" t="s">
@@ -3583,6 +3731,21 @@
       <c r="L29" s="2" t="n">
         <f aca="false">IF(H29&lt;I29,H29, I29)</f>
         <v>0.779999999999973</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">COUNTIF($K$2:$K$452,"&gt;"&amp;M29)</f>
+        <v>19</v>
+      </c>
+      <c r="P29" s="4" t="n">
+        <f aca="false">N29 / $O$3</f>
+        <v>0.0421286031042129</v>
+      </c>
+      <c r="R29" s="4" t="n">
+        <f aca="false">N29 / N26</f>
+        <v>0.730769230769231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
@@ -21792,8 +21955,8 @@
   </sheetPr>
   <dimension ref="A1:P452"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A361" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="J417" activeCellId="0" pane="topLeft" sqref="J417"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>

</xml_diff>